<commit_message>
added missing healthCondition field
</commit_message>
<xml_diff>
--- a/data/2024_05_21_RepoMetaCuration.xlsx
+++ b/data/2024_05_21_RepoMetaCuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtsueng\Anaconda3\envs\nde\nde_meta_batch_converter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8EA1B4-33E4-4DA4-A757-2CFFB643020C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445BFB84-15BB-4D13-B00B-07027F2D2164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="15120" windowHeight="8700" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1848" yWindow="1848" windowWidth="15120" windowHeight="8700" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resource_base" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1687" uniqueCount="572">
   <si>
     <t>name</t>
   </si>
@@ -1789,7 +1789,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="###0"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1907,6 +1907,13 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1925,10 +1932,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1961,8 +1969,10 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9698,9 +9708,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E140"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112:D112"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -11073,13 +11085,13 @@
     </row>
     <row r="112" spans="1:4" ht="14.4">
       <c r="A112" s="6" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B112" s="22" t="s">
-        <v>412</v>
-      </c>
-      <c r="D112" s="8" t="s">
-        <v>539</v>
+        <v>397</v>
+      </c>
+      <c r="D112" s="24" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="14.4">
@@ -11090,7 +11102,7 @@
         <v>412</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="14.4">
@@ -11101,7 +11113,7 @@
         <v>412</v>
       </c>
       <c r="D114" s="8" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="14.4">
@@ -11112,7 +11124,7 @@
         <v>412</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="14.4">
@@ -11123,18 +11135,18 @@
         <v>412</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="14.4">
       <c r="A117" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B117" s="9" t="s">
-        <v>393</v>
+      <c r="B117" s="22" t="s">
+        <v>412</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="14.4">
@@ -11145,7 +11157,7 @@
         <v>393</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="14.4">
@@ -11156,7 +11168,7 @@
         <v>393</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="14.4">
@@ -11164,10 +11176,10 @@
         <v>40</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>430</v>
+        <v>546</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="14.4">
@@ -11175,10 +11187,10 @@
         <v>40</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>547</v>
+        <v>430</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="14.4">
@@ -11186,10 +11198,10 @@
         <v>40</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="14.4">
@@ -11197,10 +11209,10 @@
         <v>40</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>397</v>
+        <v>405</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="14.4">
@@ -11211,7 +11223,7 @@
         <v>397</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="14.4">
@@ -11222,7 +11234,7 @@
         <v>397</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="14.4">
@@ -11233,7 +11245,7 @@
         <v>397</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="14.4">
@@ -11244,7 +11256,7 @@
         <v>397</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="14.4">
@@ -11255,7 +11267,7 @@
         <v>397</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="14.4">
@@ -11263,10 +11275,10 @@
         <v>40</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="14.4">
@@ -11274,10 +11286,10 @@
         <v>40</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="14.4">
@@ -11285,10 +11297,10 @@
         <v>40</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D131" s="8" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="14.4">
@@ -11296,10 +11308,10 @@
         <v>40</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="14.4">
@@ -11307,10 +11319,10 @@
         <v>40</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="14.4">
@@ -11321,7 +11333,7 @@
         <v>403</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="14.4">
@@ -11332,7 +11344,7 @@
         <v>403</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="14.4">
@@ -11340,10 +11352,10 @@
         <v>40</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="14.4">
@@ -11354,14 +11366,25 @@
         <v>405</v>
       </c>
       <c r="D137" s="8" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="14.4">
+      <c r="A138" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="D138" s="8" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" ht="14.4">
-      <c r="A138" s="6"/>
     </row>
     <row r="139" spans="1:4" ht="14.4">
       <c r="A139" s="6"/>
+    </row>
+    <row r="140" spans="1:4" ht="14.4">
+      <c r="A140" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -11585,60 +11608,63 @@
     <hyperlink ref="D110" r:id="rId218" xr:uid="{00000000-0004-0000-0500-0000D9000000}"/>
     <hyperlink ref="A111" r:id="rId219" location="/" xr:uid="{00000000-0004-0000-0500-0000DA000000}"/>
     <hyperlink ref="D111" r:id="rId220" xr:uid="{00000000-0004-0000-0500-0000DB000000}"/>
-    <hyperlink ref="A112" r:id="rId221" xr:uid="{00000000-0004-0000-0500-0000DC000000}"/>
-    <hyperlink ref="D112" r:id="rId222" xr:uid="{00000000-0004-0000-0500-0000DD000000}"/>
-    <hyperlink ref="A113" r:id="rId223" xr:uid="{00000000-0004-0000-0500-0000DE000000}"/>
-    <hyperlink ref="D113" r:id="rId224" xr:uid="{00000000-0004-0000-0500-0000DF000000}"/>
-    <hyperlink ref="A114" r:id="rId225" xr:uid="{00000000-0004-0000-0500-0000E0000000}"/>
-    <hyperlink ref="D114" r:id="rId226" xr:uid="{00000000-0004-0000-0500-0000E1000000}"/>
-    <hyperlink ref="A115" r:id="rId227" xr:uid="{00000000-0004-0000-0500-0000E2000000}"/>
-    <hyperlink ref="D115" r:id="rId228" xr:uid="{00000000-0004-0000-0500-0000E3000000}"/>
-    <hyperlink ref="A116" r:id="rId229" xr:uid="{00000000-0004-0000-0500-0000E4000000}"/>
-    <hyperlink ref="D116" r:id="rId230" xr:uid="{00000000-0004-0000-0500-0000E5000000}"/>
-    <hyperlink ref="A117" r:id="rId231" xr:uid="{00000000-0004-0000-0500-0000E6000000}"/>
-    <hyperlink ref="D117" r:id="rId232" xr:uid="{00000000-0004-0000-0500-0000E7000000}"/>
-    <hyperlink ref="A118" r:id="rId233" xr:uid="{00000000-0004-0000-0500-0000E8000000}"/>
-    <hyperlink ref="D118" r:id="rId234" xr:uid="{00000000-0004-0000-0500-0000E9000000}"/>
-    <hyperlink ref="A119" r:id="rId235" xr:uid="{00000000-0004-0000-0500-0000EA000000}"/>
-    <hyperlink ref="D119" r:id="rId236" xr:uid="{00000000-0004-0000-0500-0000EB000000}"/>
-    <hyperlink ref="A120" r:id="rId237" xr:uid="{00000000-0004-0000-0500-0000EC000000}"/>
-    <hyperlink ref="D120" r:id="rId238" xr:uid="{00000000-0004-0000-0500-0000ED000000}"/>
-    <hyperlink ref="A121" r:id="rId239" xr:uid="{00000000-0004-0000-0500-0000EE000000}"/>
-    <hyperlink ref="D121" r:id="rId240" xr:uid="{00000000-0004-0000-0500-0000EF000000}"/>
-    <hyperlink ref="A122" r:id="rId241" xr:uid="{00000000-0004-0000-0500-0000F0000000}"/>
-    <hyperlink ref="D122" r:id="rId242" xr:uid="{00000000-0004-0000-0500-0000F1000000}"/>
-    <hyperlink ref="A123" r:id="rId243" xr:uid="{00000000-0004-0000-0500-0000F2000000}"/>
-    <hyperlink ref="D123" r:id="rId244" xr:uid="{00000000-0004-0000-0500-0000F3000000}"/>
-    <hyperlink ref="A124" r:id="rId245" xr:uid="{00000000-0004-0000-0500-0000F4000000}"/>
-    <hyperlink ref="D124" r:id="rId246" xr:uid="{00000000-0004-0000-0500-0000F5000000}"/>
-    <hyperlink ref="A125" r:id="rId247" xr:uid="{00000000-0004-0000-0500-0000F6000000}"/>
-    <hyperlink ref="D125" r:id="rId248" xr:uid="{00000000-0004-0000-0500-0000F7000000}"/>
-    <hyperlink ref="A126" r:id="rId249" xr:uid="{00000000-0004-0000-0500-0000F8000000}"/>
-    <hyperlink ref="D126" r:id="rId250" xr:uid="{00000000-0004-0000-0500-0000F9000000}"/>
-    <hyperlink ref="A127" r:id="rId251" xr:uid="{00000000-0004-0000-0500-0000FA000000}"/>
-    <hyperlink ref="D127" r:id="rId252" xr:uid="{00000000-0004-0000-0500-0000FB000000}"/>
-    <hyperlink ref="A128" r:id="rId253" xr:uid="{00000000-0004-0000-0500-0000FC000000}"/>
-    <hyperlink ref="D128" r:id="rId254" xr:uid="{00000000-0004-0000-0500-0000FD000000}"/>
-    <hyperlink ref="A129" r:id="rId255" xr:uid="{00000000-0004-0000-0500-0000FE000000}"/>
-    <hyperlink ref="D129" r:id="rId256" xr:uid="{00000000-0004-0000-0500-0000FF000000}"/>
-    <hyperlink ref="A130" r:id="rId257" xr:uid="{00000000-0004-0000-0500-000000010000}"/>
-    <hyperlink ref="D130" r:id="rId258" xr:uid="{00000000-0004-0000-0500-000001010000}"/>
-    <hyperlink ref="A131" r:id="rId259" xr:uid="{00000000-0004-0000-0500-000002010000}"/>
-    <hyperlink ref="D131" r:id="rId260" xr:uid="{00000000-0004-0000-0500-000003010000}"/>
-    <hyperlink ref="A132" r:id="rId261" xr:uid="{00000000-0004-0000-0500-000004010000}"/>
-    <hyperlink ref="D132" r:id="rId262" xr:uid="{00000000-0004-0000-0500-000005010000}"/>
-    <hyperlink ref="A133" r:id="rId263" xr:uid="{00000000-0004-0000-0500-000006010000}"/>
-    <hyperlink ref="D133" r:id="rId264" xr:uid="{00000000-0004-0000-0500-000007010000}"/>
-    <hyperlink ref="A134" r:id="rId265" xr:uid="{00000000-0004-0000-0500-000008010000}"/>
-    <hyperlink ref="D134" r:id="rId266" xr:uid="{00000000-0004-0000-0500-000009010000}"/>
-    <hyperlink ref="A135" r:id="rId267" xr:uid="{00000000-0004-0000-0500-00000A010000}"/>
-    <hyperlink ref="D135" r:id="rId268" xr:uid="{00000000-0004-0000-0500-00000B010000}"/>
-    <hyperlink ref="A136" r:id="rId269" xr:uid="{00000000-0004-0000-0500-00000C010000}"/>
-    <hyperlink ref="D136" r:id="rId270" xr:uid="{00000000-0004-0000-0500-00000D010000}"/>
-    <hyperlink ref="A137" r:id="rId271" xr:uid="{00000000-0004-0000-0500-00000E010000}"/>
-    <hyperlink ref="D137" r:id="rId272" xr:uid="{00000000-0004-0000-0500-00000F010000}"/>
+    <hyperlink ref="A113" r:id="rId221" xr:uid="{00000000-0004-0000-0500-0000DC000000}"/>
+    <hyperlink ref="D113" r:id="rId222" xr:uid="{00000000-0004-0000-0500-0000DD000000}"/>
+    <hyperlink ref="A114" r:id="rId223" xr:uid="{00000000-0004-0000-0500-0000DE000000}"/>
+    <hyperlink ref="D114" r:id="rId224" xr:uid="{00000000-0004-0000-0500-0000DF000000}"/>
+    <hyperlink ref="A115" r:id="rId225" xr:uid="{00000000-0004-0000-0500-0000E0000000}"/>
+    <hyperlink ref="D115" r:id="rId226" xr:uid="{00000000-0004-0000-0500-0000E1000000}"/>
+    <hyperlink ref="A116" r:id="rId227" xr:uid="{00000000-0004-0000-0500-0000E2000000}"/>
+    <hyperlink ref="D116" r:id="rId228" xr:uid="{00000000-0004-0000-0500-0000E3000000}"/>
+    <hyperlink ref="A117" r:id="rId229" xr:uid="{00000000-0004-0000-0500-0000E4000000}"/>
+    <hyperlink ref="D117" r:id="rId230" xr:uid="{00000000-0004-0000-0500-0000E5000000}"/>
+    <hyperlink ref="A118" r:id="rId231" xr:uid="{00000000-0004-0000-0500-0000E6000000}"/>
+    <hyperlink ref="D118" r:id="rId232" xr:uid="{00000000-0004-0000-0500-0000E7000000}"/>
+    <hyperlink ref="A119" r:id="rId233" xr:uid="{00000000-0004-0000-0500-0000E8000000}"/>
+    <hyperlink ref="D119" r:id="rId234" xr:uid="{00000000-0004-0000-0500-0000E9000000}"/>
+    <hyperlink ref="A120" r:id="rId235" xr:uid="{00000000-0004-0000-0500-0000EA000000}"/>
+    <hyperlink ref="D120" r:id="rId236" xr:uid="{00000000-0004-0000-0500-0000EB000000}"/>
+    <hyperlink ref="A121" r:id="rId237" xr:uid="{00000000-0004-0000-0500-0000EC000000}"/>
+    <hyperlink ref="D121" r:id="rId238" xr:uid="{00000000-0004-0000-0500-0000ED000000}"/>
+    <hyperlink ref="A122" r:id="rId239" xr:uid="{00000000-0004-0000-0500-0000EE000000}"/>
+    <hyperlink ref="D122" r:id="rId240" xr:uid="{00000000-0004-0000-0500-0000EF000000}"/>
+    <hyperlink ref="A123" r:id="rId241" xr:uid="{00000000-0004-0000-0500-0000F0000000}"/>
+    <hyperlink ref="D123" r:id="rId242" xr:uid="{00000000-0004-0000-0500-0000F1000000}"/>
+    <hyperlink ref="A124" r:id="rId243" xr:uid="{00000000-0004-0000-0500-0000F2000000}"/>
+    <hyperlink ref="D124" r:id="rId244" xr:uid="{00000000-0004-0000-0500-0000F3000000}"/>
+    <hyperlink ref="A125" r:id="rId245" xr:uid="{00000000-0004-0000-0500-0000F4000000}"/>
+    <hyperlink ref="D125" r:id="rId246" xr:uid="{00000000-0004-0000-0500-0000F5000000}"/>
+    <hyperlink ref="A126" r:id="rId247" xr:uid="{00000000-0004-0000-0500-0000F6000000}"/>
+    <hyperlink ref="D126" r:id="rId248" xr:uid="{00000000-0004-0000-0500-0000F7000000}"/>
+    <hyperlink ref="A127" r:id="rId249" xr:uid="{00000000-0004-0000-0500-0000F8000000}"/>
+    <hyperlink ref="D127" r:id="rId250" xr:uid="{00000000-0004-0000-0500-0000F9000000}"/>
+    <hyperlink ref="A128" r:id="rId251" xr:uid="{00000000-0004-0000-0500-0000FA000000}"/>
+    <hyperlink ref="D128" r:id="rId252" xr:uid="{00000000-0004-0000-0500-0000FB000000}"/>
+    <hyperlink ref="A129" r:id="rId253" xr:uid="{00000000-0004-0000-0500-0000FC000000}"/>
+    <hyperlink ref="D129" r:id="rId254" xr:uid="{00000000-0004-0000-0500-0000FD000000}"/>
+    <hyperlink ref="A130" r:id="rId255" xr:uid="{00000000-0004-0000-0500-0000FE000000}"/>
+    <hyperlink ref="D130" r:id="rId256" xr:uid="{00000000-0004-0000-0500-0000FF000000}"/>
+    <hyperlink ref="A131" r:id="rId257" xr:uid="{00000000-0004-0000-0500-000000010000}"/>
+    <hyperlink ref="D131" r:id="rId258" xr:uid="{00000000-0004-0000-0500-000001010000}"/>
+    <hyperlink ref="A132" r:id="rId259" xr:uid="{00000000-0004-0000-0500-000002010000}"/>
+    <hyperlink ref="D132" r:id="rId260" xr:uid="{00000000-0004-0000-0500-000003010000}"/>
+    <hyperlink ref="A133" r:id="rId261" xr:uid="{00000000-0004-0000-0500-000004010000}"/>
+    <hyperlink ref="D133" r:id="rId262" xr:uid="{00000000-0004-0000-0500-000005010000}"/>
+    <hyperlink ref="A134" r:id="rId263" xr:uid="{00000000-0004-0000-0500-000006010000}"/>
+    <hyperlink ref="D134" r:id="rId264" xr:uid="{00000000-0004-0000-0500-000007010000}"/>
+    <hyperlink ref="A135" r:id="rId265" xr:uid="{00000000-0004-0000-0500-000008010000}"/>
+    <hyperlink ref="D135" r:id="rId266" xr:uid="{00000000-0004-0000-0500-000009010000}"/>
+    <hyperlink ref="A136" r:id="rId267" xr:uid="{00000000-0004-0000-0500-00000A010000}"/>
+    <hyperlink ref="D136" r:id="rId268" xr:uid="{00000000-0004-0000-0500-00000B010000}"/>
+    <hyperlink ref="A137" r:id="rId269" xr:uid="{00000000-0004-0000-0500-00000C010000}"/>
+    <hyperlink ref="D137" r:id="rId270" xr:uid="{00000000-0004-0000-0500-00000D010000}"/>
+    <hyperlink ref="A138" r:id="rId271" xr:uid="{00000000-0004-0000-0500-00000E010000}"/>
+    <hyperlink ref="D138" r:id="rId272" xr:uid="{00000000-0004-0000-0500-00000F010000}"/>
+    <hyperlink ref="D112" r:id="rId273" xr:uid="{A5180A1C-F3E4-45B1-8AF0-38BD6B2AD30E}"/>
+    <hyperlink ref="A112" r:id="rId274" location="/" xr:uid="{B62568E1-018B-43D3-B753-05BD665C3B36}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId275"/>
 </worksheet>
 </file>
 
@@ -11649,7 +11675,7 @@
   </sheetPr>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>